<commit_message>
Updated PG progress in tracker. Updated tasklist presentation assignments.
</commit_message>
<xml_diff>
--- a/FinalProject/Group3FinalTodoList.xlsx
+++ b/FinalProject/Group3FinalTodoList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuan\OneDrive\Documents\Github\CSCI381-DataModeling-Group3\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\381DataModeling\Group3\CSCI381-DataModeling-Group3\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2127A696-44AF-48FE-AF50-F1A8C0813595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48E8230-67BF-4685-99DE-75A8C0D3041D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="2250" windowWidth="17280" windowHeight="12735" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ralph Granata" sheetId="1" r:id="rId1"/>
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -1438,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F8EC82-3D7B-4B35-8BCF-93C71E414EE5}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -2286,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7F7114-971E-49E2-8EA2-0E1816A122F1}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated self presentation progress in tracker.
</commit_message>
<xml_diff>
--- a/FinalProject/Group3FinalTodoList.xlsx
+++ b/FinalProject/Group3FinalTodoList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\381DataModeling\Group3\CSCI381-DataModeling-Group3\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48E8230-67BF-4685-99DE-75A8C0D3041D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FCCD4F-3A54-420F-AD97-F30CA1955A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1305" yWindow="2250" windowWidth="17280" windowHeight="12735" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>

</xml_diff>